<commit_message>
Added field modifications for showing and creating
</commit_message>
<xml_diff>
--- a/ConsumableReceivedLogs.xlsx
+++ b/ConsumableReceivedLogs.xlsx
@@ -413,14 +413,167 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>ProductName</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>LOT</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>DateReceived</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>DateReceivedIni</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>DemoProd1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>LOT-001</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2026-02-02</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>20260202</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>6</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>7</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Hey</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>